<commit_message>
[WEek 5] Renamed the query by TotalsByProduct
Signed-off-by: Synthia Islam <synthia.mist@gmail.com>
</commit_message>
<xml_diff>
--- a/Synthia_S375728/Week_5/Power-Query/Power-query.xlsx
+++ b/Synthia_S375728/Week_5/Power-Query/Power-query.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Professional\Aus\CDU\Class\Semester 4 2025\PRT681-Software_Practice\PRT681_S2025_developers\Synthia_S375728\Week_5\Power-Query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A33C9-778C-4E79-A643-1F718BAFB0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48378AF-1D1F-4434-AC11-06D1AA7A6B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5532" yWindow="2172" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesQuery" sheetId="2" r:id="rId1"/>
     <sheet name="ApplesOnly" sheetId="4" r:id="rId2"/>
-    <sheet name="Query1" sheetId="3" r:id="rId3"/>
+    <sheet name="TotalsByProduct " sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">SalesQuery!$A$1:$E$5</definedName>
-    <definedName name="ExternalData_2" localSheetId="2" hidden="1">Query1!$A$1:$D$4</definedName>
+    <definedName name="ExternalData_2" localSheetId="2" hidden="1">'TotalsByProduct '!$A$1:$D$4</definedName>
     <definedName name="ExternalData_3" localSheetId="1" hidden="1">ApplesOnly!$A$1:$E$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -127,10 +127,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -196,8 +196,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{511F67FD-CD4B-47F0-ABA8-F314F8B6DDC7}" name="SalesData" displayName="SalesData" ref="A1:E5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E5" xr:uid="{511F67FD-CD4B-47F0-ABA8-F314F8B6DDC7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{859C8CD1-A80A-449F-9872-D1916EFAE02D}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{B7873075-7A2B-4321-A2EB-5DDDA606F529}" uniqueName="2" name="Product" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{859C8CD1-A80A-449F-9872-D1916EFAE02D}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B7873075-7A2B-4321-A2EB-5DDDA606F529}" uniqueName="2" name="Product" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{5442D051-8798-4704-A8C9-E3211077537B}" uniqueName="3" name="Quantity" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{98099979-239A-4F71-96A8-C9455C99A16B}" uniqueName="4" name="Price" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{CCE9B401-0510-4CCC-B028-C61C2CA98F6E}" uniqueName="5" name="TotalAmount" queryTableFieldId="5"/>
@@ -210,8 +210,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{71EE93FC-E38A-4BC6-8530-A0BC6C483998}" name="ApplesOnly" displayName="ApplesOnly" ref="A1:E3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E3" xr:uid="{71EE93FC-E38A-4BC6-8530-A0BC6C483998}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{64A019D4-FB10-4607-8F5B-6D44E6E18B48}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{02F33E41-92CA-4D1D-ABF8-A10226946346}" uniqueName="2" name="Product" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{64A019D4-FB10-4607-8F5B-6D44E6E18B48}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{02F33E41-92CA-4D1D-ABF8-A10226946346}" uniqueName="2" name="Product" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{1779F8BC-EED0-4628-A6C0-8677D29ED691}" uniqueName="3" name="Quantity" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{7F5235BE-33EA-448C-92D3-76C7BC46B7D0}" uniqueName="4" name="Price" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{9D137DF3-3521-43C2-BAFE-6B4A1C409691}" uniqueName="5" name="TotalAmount" queryTableFieldId="5"/>
@@ -224,7 +224,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A5CB8721-217D-4842-82A1-9330A36B75CF}" name="TotalsByProduct" displayName="TotalsByProduct" ref="A1:D4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{A5CB8721-217D-4842-82A1-9330A36B75CF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5ABFA997-DD11-4ED7-8BA6-235CFE1F0BEA}" uniqueName="1" name="Product" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5ABFA997-DD11-4ED7-8BA6-235CFE1F0BEA}" uniqueName="1" name="Product" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{EC7CF01A-4154-4C57-89B6-7CAC726A3724}" uniqueName="2" name="TotalQuantity" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{A7347BF1-4ADE-4983-882A-081308C29B1A}" uniqueName="3" name="TotalSales" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A1BE57B6-58B1-4641-A557-1D6F46CCCF2D}" uniqueName="4" name="Transactions" queryTableFieldId="4"/>

</xml_diff>